<commit_message>
Test interchanging and combined models
</commit_message>
<xml_diff>
--- a/Data/EN_model/Model_log.xlsx
+++ b/Data/EN_model/Model_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hungyunlu/Library/CloudStorage/Box-Box/Hung-Yun Lu Research File/Projects/FSCV/Script/Data/EN_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC763155-3A79-AA4B-88A3-DCC491051668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0938B427-509F-F340-9670-EDE29DF83D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="500" windowWidth="28260" windowHeight="16880" xr2:uid="{00FF9625-BC49-7B43-80E8-E947B345DFAB}"/>
+    <workbookView xWindow="260" yWindow="500" windowWidth="28260" windowHeight="16880" activeTab="5" xr2:uid="{00FF9625-BC49-7B43-80E8-E947B345DFAB}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="11" r:id="rId1"/>
@@ -518,9 +518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C74FDA7-245B-2D4E-ADC1-47C2408CAA63}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -1311,7 +1309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C571471E-E123-7B47-B644-43083ADA9EDA}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>

</xml_diff>